<commit_message>
added some new formatting
</commit_message>
<xml_diff>
--- a/bonus/bonus_points.xlsx
+++ b/bonus/bonus_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bonus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA301D43-B3DD-0340-A69D-CFEDCD656D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CAB8E0-B13C-1E48-B3D6-9F2010720569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,14 +457,16 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="21.83203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
corrected one highest checkout
</commit_message>
<xml_diff>
--- a/bonus/bonus_points.xlsx
+++ b/bonus/bonus_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bonus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CAB8E0-B13C-1E48-B3D6-9F2010720569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DE909B-47F4-5149-B52D-60F37F1A6E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
     <t>74</t>
   </si>
   <si>
-    <t>70</t>
+    <t>97</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
added round 6 with some bug fixes
</commit_message>
<xml_diff>
--- a/bonus/bonus_points.xlsx
+++ b/bonus/bonus_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bonus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DE909B-47F4-5149-B52D-60F37F1A6E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0345BDC-4818-B446-851D-932DC389DCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Berci Pusztai</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>97</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>101</t>
   </si>
 </sst>
 </file>
@@ -454,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -567,6 +573,20 @@
         <v>17</v>
       </c>
     </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added round 8 results
</commit_message>
<xml_diff>
--- a/bonus/bonus_points.xlsx
+++ b/bonus/bonus_points.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="+vDK7Fx/WFIFt5rDS+UX2zJxPh55lmVqb2P31uxGry0="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="xUpxGApiPF7qIGvVRV+5ognS6LD5pwbjpVWK2GtqqNM="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Season</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>93</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Ákos Szevtnik</t>
+  </si>
+  <si>
+    <t>71</t>
   </si>
 </sst>
 </file>
@@ -645,16 +654,16 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="1"/>
@@ -681,10 +690,18 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>

</xml_diff>

<commit_message>
round 10 results added
</commit_message>
<xml_diff>
--- a/bonus/bonus_points.xlsx
+++ b/bonus/bonus_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\R\darts-statistics\bonus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC648644-D3B7-43C2-A338-E5BC00A97F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C487E7-83ED-45CF-8AF0-0A65A484F208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>Season</t>
   </si>
@@ -113,6 +113,12 @@
   <si>
     <t>105</t>
   </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
 </sst>
 </file>
 
@@ -129,6 +135,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -372,7 +379,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -782,10 +789,18 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>

</xml_diff>

<commit_message>
added round 12 results
</commit_message>
<xml_diff>
--- a/bonus/bonus_points.xlsx
+++ b/bonus/bonus_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\R\darts-statistics\bonus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C487E7-83ED-45CF-8AF0-0A65A484F208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174254C0-9825-425F-B693-E82027A42D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Season</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>116</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>90</t>
   </si>
 </sst>
 </file>
@@ -379,7 +385,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -825,10 +831,18 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>

</xml_diff>

<commit_message>
added 2025 round 3 results
</commit_message>
<xml_diff>
--- a/bonus/bonus_points.xlsx
+++ b/bonus/bonus_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bonus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25DACA8-2D74-BC4D-BE68-FCD42E1B93A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D07CB5-3AE1-F441-99F8-AE6A1B150FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
   <si>
     <t>Season</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>96</t>
+  </si>
+  <si>
+    <t>Tomi Csánk</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>Laci Ferenczi</t>
   </si>
 </sst>
 </file>
@@ -401,7 +410,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -991,10 +1000,18 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1019,10 +1036,18 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>

</xml_diff>

<commit_message>
added 2025 round 4 results
</commit_message>
<xml_diff>
--- a/bonus/bonus_points.xlsx
+++ b/bonus/bonus_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bonus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D07CB5-3AE1-F441-99F8-AE6A1B150FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97319E0C-5F65-1049-A9A7-2F7B7C90BA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>Season</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Laci Ferenczi</t>
+  </si>
+  <si>
+    <t>111</t>
   </si>
 </sst>
 </file>
@@ -1072,10 +1075,18 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>

</xml_diff>

<commit_message>
added 2025 round 6 results
</commit_message>
<xml_diff>
--- a/bonus/bonus_points.xlsx
+++ b/bonus/bonus_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bonus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D39977-7560-9C41-90A5-8DF72A08F011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BEC9C2-9A48-834D-869D-F7CEC9AFE850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
     <t>Season</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>109</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1150,10 +1153,18 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1178,10 +1189,18 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>

</xml_diff>

<commit_message>
added 2025 round 7 results
</commit_message>
<xml_diff>
--- a/bonus/bonus_points.xlsx
+++ b/bonus/bonus_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bonus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BEC9C2-9A48-834D-869D-F7CEC9AFE850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6BAC6B-CCA1-B34B-ADF4-2A73920F0922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
   <si>
     <t>Season</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>100</t>
+  </si>
+  <si>
+    <t>125</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1225,10 +1228,18 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>

</xml_diff>

<commit_message>
added 2025 round 9 results
</commit_message>
<xml_diff>
--- a/bonus/bonus_points.xlsx
+++ b/bonus/bonus_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bonus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4CCCD2-9816-FF4D-8B68-0A691B9907A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA7D17D-E978-4C4A-BDB8-94A0878DC968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
   <si>
     <t>Season</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Dani Pusztai</t>
+  </si>
+  <si>
+    <t>143</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1342,10 +1345,18 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>

</xml_diff>

<commit_message>
added 2026 round 1 results
</commit_message>
<xml_diff>
--- a/bonus/bonus_points.xlsx
+++ b/bonus/bonus_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/bonus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8992BC2-F881-1546-AF51-15DCC43B750F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A69CD6-FD7F-0545-A4AB-FAB597F8521D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
   <si>
     <t>Season</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>82</t>
+  </si>
+  <si>
+    <t>2026</t>
   </si>
 </sst>
 </file>
@@ -434,7 +437,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1456,10 +1459,18 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>

</xml_diff>